<commit_message>
made some changes to the sprints
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint3/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint3/Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhertz/Documents/subjects/SE/ganttproject/Project/Phase 2/Sprint3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1DCDA58-02B9-4C77-AB44-7BC07E30197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198A24A9-8592-1742-A448-80A14545F08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,26 +50,26 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Debugs</t>
-  </si>
-  <si>
-    <t>Correct bugs</t>
-  </si>
-  <si>
     <t>Analyse how to implement features 1 (Ricardo)</t>
   </si>
   <si>
     <t>Analyse how to implement features 2 (Iago,James,Joao,Francisco)</t>
   </si>
   <si>
-    <t>Make java program to encapsulate tasks</t>
+    <t>Debugs (Iago)</t>
+  </si>
+  <si>
+    <t>Correct bugs (Iago)</t>
+  </si>
+  <si>
+    <t>Make java program to encapsulate tasks (Iago)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,18 +418,18 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,39 +443,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -483,7 +483,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,39 +497,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>

</xml_diff>